<commit_message>
update cascade births with meaningful names
</commit_message>
<xml_diff>
--- a/data/databook-simple-cascadeBirths.xlsx
+++ b/data/databook-simple-cascadeBirths.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14440" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="25365" windowHeight="14445" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -21,11 +16,8 @@
     <sheet name="Epidemic Characteristics" sheetId="7" r:id="rId7"/>
     <sheet name="Cascade Parameters" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -48,12 +40,6 @@
     <t>Maximum Age</t>
   </si>
   <si>
-    <t>Population 1</t>
-  </si>
-  <si>
-    <t>Population 2</t>
-  </si>
-  <si>
     <t>Aging</t>
   </si>
   <si>
@@ -148,6 +134,18 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>General Population</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>GEN</t>
   </si>
 </sst>
 </file>
@@ -490,12 +488,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="15.6640625" customWidth="1"/>
+    <col min="1" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -514,11 +512,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="str">
-        <f>LEFT(A2,3)&amp;"1"</f>
-        <v>Pop1</v>
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -529,11 +526,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="str">
-        <f>LEFT(A3,3)&amp;"2"</f>
-        <v>Pop2</v>
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -555,102 +551,102 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C1" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C5" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C9" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Population Definitions'!$B$2</f>
-        <v>Pop1</v>
+        <v>SAC</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>'Population Definitions'!$B$3</f>
-        <v>Pop2</v>
+        <v>GEN</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -702,11 +698,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -715,10 +711,10 @@
         <v>Migration Type 1</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1">
         <v>2000</v>
@@ -827,10 +823,10 @@
         <v>Migration Type 2</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>2000</v>
@@ -956,25 +952,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>2000</v>
@@ -1028,44 +1024,44 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <f>IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,200000,"N.A.")</f>
         <v>200000</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>IF(SUMPRODUCT(--(E3:T3&lt;&gt;""))=0,200000,"N.A.")</f>
         <v>200000</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -1119,61 +1115,54 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="str">
         <f>IF(SUMPRODUCT(--(E6:T6&lt;&gt;""))=0,100,"N.A.")</f>
         <v>N.A.</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>400</v>
       </c>
       <c r="F6">
-        <v>5000</v>
-      </c>
-      <c r="G6" s="1">
-        <v>60000</v>
+        <v>500</v>
+      </c>
+      <c r="G6">
+        <v>600</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>4000</v>
+        <v>800</v>
+      </c>
+      <c r="J6">
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IF(SUMPRODUCT(--(E7:T7&lt;&gt;""))=0,100,"N.A.")</f>
-        <v>N.A.</v>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1">
-        <v>70000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>50000</v>
-      </c>
-      <c r="G7" s="1">
-        <v>60000</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -1200,21 +1189,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>2000</v>
@@ -1268,44 +1257,44 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <f>IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>IF(SUMPRODUCT(--(E3:T3&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -1359,44 +1348,44 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <f>IF(SUMPRODUCT(--(E6:T6&lt;&gt;""))=0,10000,"N.A.")</f>
         <v>10000</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <f>IF(SUMPRODUCT(--(E7:T7&lt;&gt;""))=0,10000,"N.A.")</f>
         <v>10000</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>2000</v>
@@ -1450,44 +1439,44 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <f>IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <f>IF(SUMPRODUCT(--(E11:T11&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>2000</v>
@@ -1541,44 +1530,44 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <f>IF(SUMPRODUCT(--(E14:T14&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f>IF(SUMPRODUCT(--(E15:T15&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>2000</v>
@@ -1632,44 +1621,44 @@
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <f>IF(SUMPRODUCT(--(E18:T18&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <f>IF(SUMPRODUCT(--(E19:T19&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>2000</v>
@@ -1723,33 +1712,33 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <f>IF(SUMPRODUCT(--(E22:T22&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <f>IF(SUMPRODUCT(--(E23:T23&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1801,21 +1790,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>2000</v>
@@ -1869,44 +1858,44 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f>IF(SUMPRODUCT(--(E3:T3&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -1960,33 +1949,33 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f>IF(SUMPRODUCT(--(E6:T6&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <f>IF(SUMPRODUCT(--(E7:T7&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2012,23 +2001,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>2000</v>
@@ -2082,33 +2073,33 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f>IF(SUMPRODUCT(--(E3:T3&lt;&gt;""))=0,0,"N.A.")</f>
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2128,23 +2119,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>2000</v>
@@ -2198,44 +2189,44 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <f>IF(SUMPRODUCT(--(E3:T3&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2000</v>
@@ -2289,44 +2280,44 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f>IF(SUMPRODUCT(--(E6:T6&lt;&gt;""))=0,0.02,"N.A.")</f>
         <v>0.02</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <f>IF(SUMPRODUCT(--(E7:T7&lt;&gt;""))=0,0.02,"N.A.")</f>
         <v>0.02</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>2000</v>
@@ -2380,44 +2371,44 @@
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f>IF(SUMPRODUCT(--(E11:T11&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>2000</v>
@@ -2471,44 +2462,44 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <f>IF(SUMPRODUCT(--(E14:T14&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <f>IF(SUMPRODUCT(--(E15:T15&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>2000</v>
@@ -2562,44 +2553,44 @@
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <f>IF(SUMPRODUCT(--(E18:T18&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <f>IF(SUMPRODUCT(--(E19:T19&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <v>2000</v>
@@ -2653,44 +2644,44 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <f>IF(SUMPRODUCT(--(E22:T22&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <f>IF(SUMPRODUCT(--(E23:T23&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E25">
         <v>2000</v>
@@ -2744,44 +2735,44 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <f>IF(SUMPRODUCT(--(E26:T26&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <f>IF(SUMPRODUCT(--(E27:T27&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E29">
         <v>2000</v>
@@ -2835,44 +2826,44 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <f>IF(SUMPRODUCT(--(E30:T30&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <f>IF(SUMPRODUCT(--(E31:T31&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E33">
         <v>2000</v>
@@ -2926,44 +2917,44 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C34">
         <f>IF(SUMPRODUCT(--(E34:T34&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <f>IF(SUMPRODUCT(--(E35:T35&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E37">
         <v>2000</v>
@@ -3017,44 +3008,44 @@
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38">
         <f>IF(SUMPRODUCT(--(E38:T38&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <f>IF(SUMPRODUCT(--(E39:T39&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E41">
         <v>2000</v>
@@ -3105,36 +3096,36 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>'Population Definitions'!$A$2</f>
-        <v>Population 1</v>
+        <v>Children</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C42">
         <f>IF(SUMPRODUCT(--(E42:T42&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>'Population Definitions'!$A$3</f>
-        <v>Population 2</v>
+        <v>General Population</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C43">
         <f>IF(SUMPRODUCT(--(E43:T43&lt;&gt;""))=0,0.01,"N.A.")</f>
         <v>0.01</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>